<commit_message>
updated hyp gen data
</commit_message>
<xml_diff>
--- a/refined-hyp-data-3.xlsx
+++ b/refined-hyp-data-3.xlsx
@@ -31,10 +31,10 @@
     <t>P(O|H)</t>
   </si>
   <si>
+    <t>P(H|O)</t>
+  </si>
+  <si>
     <t>Best Explanation (flipped)</t>
-  </si>
-  <si>
-    <t>P(H|O)</t>
   </si>
   <si>
     <t>['B1']</t>
@@ -1115,11 +1115,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2">
+      <c r="G2">
         <v>0.0822123787580261</v>
+      </c>
+      <c r="H2" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1141,11 +1141,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>228</v>
-      </c>
-      <c r="H3">
+      <c r="G3">
         <v>0.06790001332745053</v>
+      </c>
+      <c r="H3" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1167,11 +1167,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>228</v>
-      </c>
-      <c r="H4">
+      <c r="G4">
         <v>0.05468171459519593</v>
+      </c>
+      <c r="H4" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1193,11 +1193,11 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>0.2629514961735958</v>
+      </c>
+      <c r="H5" t="s">
         <v>229</v>
-      </c>
-      <c r="H5">
-        <v>0.2629514961735958</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1219,11 +1219,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>0.04547141860584613</v>
+      </c>
+      <c r="H6" t="s">
         <v>229</v>
-      </c>
-      <c r="H6">
-        <v>0.04547141860584613</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1245,11 +1245,11 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
-        <v>228</v>
-      </c>
-      <c r="H7">
+      <c r="G7">
         <v>0.06063476235243403</v>
+      </c>
+      <c r="H7" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1271,11 +1271,11 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
-        <v>228</v>
-      </c>
-      <c r="H8">
+      <c r="G8">
         <v>0.04030129522014882</v>
+      </c>
+      <c r="H8" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1297,11 +1297,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
-        <v>228</v>
-      </c>
-      <c r="H9">
+      <c r="G9">
         <v>0.086901769271174</v>
+      </c>
+      <c r="H9" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1323,11 +1323,11 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
-        <v>228</v>
-      </c>
-      <c r="H10">
+      <c r="G10">
         <v>0.06354147988076518</v>
+      </c>
+      <c r="H10" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1349,11 +1349,11 @@
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>0.2629514961735958</v>
+      </c>
+      <c r="H11" t="s">
         <v>229</v>
-      </c>
-      <c r="H11">
-        <v>0.2629514961735958</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1375,11 +1375,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12">
+        <v>0.04547141860584613</v>
+      </c>
+      <c r="H12" t="s">
         <v>229</v>
-      </c>
-      <c r="H12">
-        <v>0.04547141860584613</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1401,11 +1401,11 @@
       <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13" t="s">
-        <v>228</v>
-      </c>
-      <c r="H13">
+      <c r="G13">
         <v>0.07745045519474988</v>
+      </c>
+      <c r="H13" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1427,11 +1427,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
-        <v>228</v>
-      </c>
-      <c r="H14">
+      <c r="G14">
         <v>0.04561744588877638</v>
+      </c>
+      <c r="H14" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1453,11 +1453,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
-        <v>228</v>
-      </c>
-      <c r="H15">
+      <c r="G15">
         <v>0.06206522356065326</v>
+      </c>
+      <c r="H15" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1479,11 +1479,11 @@
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16">
+        <v>0.2629514961735958</v>
+      </c>
+      <c r="H16" t="s">
         <v>229</v>
-      </c>
-      <c r="H16">
-        <v>0.2629514961735958</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1505,11 +1505,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17">
+        <v>0.04547141860584613</v>
+      </c>
+      <c r="H17" t="s">
         <v>229</v>
-      </c>
-      <c r="H17">
-        <v>0.04547141860584613</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1531,11 +1531,11 @@
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" t="s">
-        <v>228</v>
-      </c>
-      <c r="H18">
+      <c r="G18">
         <v>0.05858210392112535</v>
+      </c>
+      <c r="H18" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1557,11 +1557,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-      <c r="G19" t="s">
-        <v>228</v>
-      </c>
-      <c r="H19">
+      <c r="G19">
         <v>0.04380767160551077</v>
+      </c>
+      <c r="H19" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1583,11 +1583,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20">
+        <v>0.268207609833135</v>
+      </c>
+      <c r="H20" t="s">
         <v>229</v>
-      </c>
-      <c r="H20">
-        <v>0.268207609833135</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1609,11 +1609,11 @@
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="G21" t="s">
-        <v>228</v>
-      </c>
-      <c r="H21">
+      <c r="G21">
         <v>0.04886924445435459</v>
+      </c>
+      <c r="H21" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1635,11 +1635,11 @@
       <c r="F22">
         <v>1</v>
       </c>
-      <c r="G22" t="s">
-        <v>228</v>
-      </c>
-      <c r="H22">
+      <c r="G22">
         <v>0.04363957256688109</v>
+      </c>
+      <c r="H22" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1661,11 +1661,11 @@
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="G23" t="s">
-        <v>228</v>
-      </c>
-      <c r="H23">
+      <c r="G23">
         <v>0.02865844532533962</v>
+      </c>
+      <c r="H23" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1687,11 +1687,11 @@
       <c r="F24">
         <v>1</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24">
+        <v>0.248596438043593</v>
+      </c>
+      <c r="H24" t="s">
         <v>229</v>
-      </c>
-      <c r="H24">
-        <v>0.248596438043593</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1713,11 +1713,11 @@
       <c r="F25">
         <v>1</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25">
+        <v>0.1954968605456482</v>
+      </c>
+      <c r="H25" t="s">
         <v>230</v>
-      </c>
-      <c r="H25">
-        <v>0.1954968605456482</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1739,11 +1739,11 @@
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26">
+        <v>0.1361480655135886</v>
+      </c>
+      <c r="H26" t="s">
         <v>231</v>
-      </c>
-      <c r="H26">
-        <v>0.1361480655135886</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1765,11 +1765,11 @@
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27">
+        <v>0.03593370716208692</v>
+      </c>
+      <c r="H27" t="s">
         <v>230</v>
-      </c>
-      <c r="H27">
-        <v>0.03593370716208692</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1791,11 +1791,11 @@
       <c r="F28">
         <v>1</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28">
+        <v>0.04202043911776646</v>
+      </c>
+      <c r="H28" t="s">
         <v>231</v>
-      </c>
-      <c r="H28">
-        <v>0.04202043911776646</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1817,11 +1817,11 @@
       <c r="F29">
         <v>1</v>
       </c>
-      <c r="G29" t="s">
-        <v>228</v>
-      </c>
-      <c r="H29">
+      <c r="G29">
         <v>0.04264444475012164</v>
+      </c>
+      <c r="H29" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1843,11 +1843,11 @@
       <c r="F30">
         <v>1</v>
       </c>
-      <c r="G30" t="s">
-        <v>228</v>
-      </c>
-      <c r="H30">
+      <c r="G30">
         <v>0.07464945633127076</v>
+      </c>
+      <c r="H30" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1869,11 +1869,11 @@
       <c r="F31">
         <v>1</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31">
+        <v>0.2629514961735958</v>
+      </c>
+      <c r="H31" t="s">
         <v>229</v>
-      </c>
-      <c r="H31">
-        <v>0.2629514961735958</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1895,11 +1895,11 @@
       <c r="F32">
         <v>1</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32">
+        <v>0.04547141860584612</v>
+      </c>
+      <c r="H32" t="s">
         <v>229</v>
-      </c>
-      <c r="H32">
-        <v>0.04547141860584612</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1921,11 +1921,11 @@
       <c r="F33">
         <v>1</v>
       </c>
-      <c r="G33" t="s">
-        <v>228</v>
-      </c>
-      <c r="H33">
+      <c r="G33">
         <v>0.07350696097347734</v>
+      </c>
+      <c r="H33" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1947,11 +1947,11 @@
       <c r="F34">
         <v>1</v>
       </c>
-      <c r="G34" t="s">
-        <v>228</v>
-      </c>
-      <c r="H34">
+      <c r="G34">
         <v>0.05030197306018955</v>
+      </c>
+      <c r="H34" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1973,11 +1973,11 @@
       <c r="F35">
         <v>1</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35">
+        <v>0.2682076098331351</v>
+      </c>
+      <c r="H35" t="s">
         <v>229</v>
-      </c>
-      <c r="H35">
-        <v>0.2682076098331351</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1999,11 +1999,11 @@
       <c r="F36">
         <v>1</v>
       </c>
-      <c r="G36" t="s">
-        <v>228</v>
-      </c>
-      <c r="H36">
+      <c r="G36">
         <v>0.05525483750915555</v>
+      </c>
+      <c r="H36" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2025,11 +2025,11 @@
       <c r="F37">
         <v>1</v>
       </c>
-      <c r="G37" t="s">
-        <v>228</v>
-      </c>
-      <c r="H37">
+      <c r="G37">
         <v>0.05290772104811078</v>
+      </c>
+      <c r="H37" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2051,11 +2051,11 @@
       <c r="F38">
         <v>1</v>
       </c>
-      <c r="G38" t="s">
-        <v>228</v>
-      </c>
-      <c r="H38">
+      <c r="G38">
         <v>0.03244283555361271</v>
+      </c>
+      <c r="H38" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2077,11 +2077,11 @@
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39">
+        <v>0.248596438043593</v>
+      </c>
+      <c r="H39" t="s">
         <v>229</v>
-      </c>
-      <c r="H39">
-        <v>0.248596438043593</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2103,11 +2103,11 @@
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40">
+        <v>0.1954968605456481</v>
+      </c>
+      <c r="H40" t="s">
         <v>230</v>
-      </c>
-      <c r="H40">
-        <v>0.1954968605456481</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2129,11 +2129,11 @@
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41">
+        <v>0.1361480655135885</v>
+      </c>
+      <c r="H41" t="s">
         <v>231</v>
-      </c>
-      <c r="H41">
-        <v>0.1361480655135885</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2155,11 +2155,11 @@
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42">
+        <v>0.03593370716208692</v>
+      </c>
+      <c r="H42" t="s">
         <v>230</v>
-      </c>
-      <c r="H42">
-        <v>0.03593370716208692</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2181,11 +2181,11 @@
       <c r="F43">
         <v>1</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43">
+        <v>0.04202043911776644</v>
+      </c>
+      <c r="H43" t="s">
         <v>231</v>
-      </c>
-      <c r="H43">
-        <v>0.04202043911776644</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2207,11 +2207,11 @@
       <c r="F44">
         <v>1</v>
       </c>
-      <c r="G44" t="s">
-        <v>228</v>
-      </c>
-      <c r="H44">
+      <c r="G44">
         <v>0.05171001288247373</v>
+      </c>
+      <c r="H44" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2233,11 +2233,11 @@
       <c r="F45">
         <v>1</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45">
+        <v>0.268207609833135</v>
+      </c>
+      <c r="H45" t="s">
         <v>229</v>
-      </c>
-      <c r="H45">
-        <v>0.268207609833135</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2259,11 +2259,11 @@
       <c r="F46">
         <v>1</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46">
+        <v>0.04638034267713199</v>
+      </c>
+      <c r="H46" t="s">
         <v>229</v>
-      </c>
-      <c r="H46">
-        <v>0.04638034267713199</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2285,11 +2285,11 @@
       <c r="F47">
         <v>1</v>
       </c>
-      <c r="G47" t="s">
-        <v>228</v>
-      </c>
-      <c r="H47">
+      <c r="G47">
         <v>0.04667334377643362</v>
+      </c>
+      <c r="H47" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2311,11 +2311,11 @@
       <c r="F48">
         <v>1</v>
       </c>
-      <c r="G48" t="s">
-        <v>228</v>
-      </c>
-      <c r="H48">
+      <c r="G48">
         <v>0.03272729337207169</v>
+      </c>
+      <c r="H48" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2337,11 +2337,11 @@
       <c r="F49">
         <v>1</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49">
+        <v>0.248596438043593</v>
+      </c>
+      <c r="H49" t="s">
         <v>229</v>
-      </c>
-      <c r="H49">
-        <v>0.248596438043593</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2363,11 +2363,11 @@
       <c r="F50">
         <v>1</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50">
+        <v>0.2140962469836062</v>
+      </c>
+      <c r="H50" t="s">
         <v>230</v>
-      </c>
-      <c r="H50">
-        <v>0.2140962469836062</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2389,11 +2389,11 @@
       <c r="F51">
         <v>1</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51">
+        <v>0.1366613794446337</v>
+      </c>
+      <c r="H51" t="s">
         <v>231</v>
-      </c>
-      <c r="H51">
-        <v>0.1366613794446337</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2415,11 +2415,11 @@
       <c r="F52">
         <v>1</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52">
+        <v>0.04046133891800937</v>
+      </c>
+      <c r="H52" t="s">
         <v>230</v>
-      </c>
-      <c r="H52">
-        <v>0.04046133891800937</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2441,11 +2441,11 @@
       <c r="F53">
         <v>1</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53">
+        <v>0.03379797915054781</v>
+      </c>
+      <c r="H53" t="s">
         <v>231</v>
-      </c>
-      <c r="H53">
-        <v>0.03379797915054781</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2467,11 +2467,11 @@
       <c r="F54">
         <v>1</v>
       </c>
-      <c r="G54" t="s">
-        <v>228</v>
-      </c>
-      <c r="H54">
+      <c r="G54">
         <v>0.04261268674073516</v>
+      </c>
+      <c r="H54" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2493,11 +2493,11 @@
       <c r="F55">
         <v>1</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55">
+        <v>0.2535656097453242</v>
+      </c>
+      <c r="H55" t="s">
         <v>229</v>
-      </c>
-      <c r="H55">
-        <v>0.2535656097453242</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2519,11 +2519,11 @@
       <c r="F56">
         <v>1</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56">
+        <v>0.1954968605456481</v>
+      </c>
+      <c r="H56" t="s">
         <v>230</v>
-      </c>
-      <c r="H56">
-        <v>0.1954968605456481</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2545,11 +2545,11 @@
       <c r="F57">
         <v>1</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57">
+        <v>0.09675141504657259</v>
+      </c>
+      <c r="H57" t="s">
         <v>231</v>
-      </c>
-      <c r="H57">
-        <v>0.09675141504657259</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2571,11 +2571,11 @@
       <c r="F58">
         <v>1</v>
       </c>
-      <c r="G58" t="s">
-        <v>228</v>
-      </c>
-      <c r="H58">
+      <c r="G58">
         <v>0.05708123659060638</v>
+      </c>
+      <c r="H58" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2597,11 +2597,11 @@
       <c r="F59">
         <v>1</v>
       </c>
-      <c r="G59" t="s">
-        <v>228</v>
-      </c>
-      <c r="H59">
+      <c r="G59">
         <v>0.03335013995169677</v>
+      </c>
+      <c r="H59" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2623,11 +2623,11 @@
       <c r="F60">
         <v>1</v>
       </c>
-      <c r="G60" t="s">
-        <v>228</v>
-      </c>
-      <c r="H60">
+      <c r="G60">
         <v>0.02553577334619476</v>
+      </c>
+      <c r="H60" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2649,11 +2649,11 @@
       <c r="F61">
         <v>1</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61">
+        <v>0.1964528901908476</v>
+      </c>
+      <c r="H61" t="s">
         <v>230</v>
-      </c>
-      <c r="H61">
-        <v>0.1964528901908476</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2675,11 +2675,11 @@
       <c r="F62">
         <v>1</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62">
+        <v>0.2297296149973507</v>
+      </c>
+      <c r="H62" t="s">
         <v>231</v>
-      </c>
-      <c r="H62">
-        <v>0.2297296149973507</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2701,11 +2701,11 @@
       <c r="F63">
         <v>1</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63">
+        <v>0.08958513629817907</v>
+      </c>
+      <c r="H63" t="s">
         <v>231</v>
-      </c>
-      <c r="H63">
-        <v>0.08958513629817907</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2727,11 +2727,11 @@
       <c r="F64">
         <v>1</v>
       </c>
-      <c r="G64" t="s">
-        <v>228</v>
-      </c>
-      <c r="H64">
+      <c r="G64">
         <v>0.01760208236291312</v>
+      </c>
+      <c r="H64" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2753,11 +2753,11 @@
       <c r="F65">
         <v>1</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65">
+        <v>0.268207609833135</v>
+      </c>
+      <c r="H65" t="s">
         <v>229</v>
-      </c>
-      <c r="H65">
-        <v>0.268207609833135</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2779,11 +2779,11 @@
       <c r="F66">
         <v>1</v>
       </c>
-      <c r="G66" t="s">
-        <v>228</v>
-      </c>
-      <c r="H66">
+      <c r="G66">
         <v>0.05228091384282959</v>
+      </c>
+      <c r="H66" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2805,11 +2805,11 @@
       <c r="F67">
         <v>1</v>
       </c>
-      <c r="G67" t="s">
-        <v>228</v>
-      </c>
-      <c r="H67">
+      <c r="G67">
         <v>0.05562363358634346</v>
+      </c>
+      <c r="H67" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2831,11 +2831,11 @@
       <c r="F68">
         <v>1</v>
       </c>
-      <c r="G68" t="s">
-        <v>228</v>
-      </c>
-      <c r="H68">
+      <c r="G68">
         <v>0.03819607002916236</v>
+      </c>
+      <c r="H68" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2857,11 +2857,11 @@
       <c r="F69">
         <v>1</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69">
+        <v>0.248596438043593</v>
+      </c>
+      <c r="H69" t="s">
         <v>229</v>
-      </c>
-      <c r="H69">
-        <v>0.248596438043593</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2883,11 +2883,11 @@
       <c r="F70">
         <v>1</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70">
+        <v>0.2140962469836062</v>
+      </c>
+      <c r="H70" t="s">
         <v>230</v>
-      </c>
-      <c r="H70">
-        <v>0.2140962469836062</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2909,11 +2909,11 @@
       <c r="F71">
         <v>1</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G71">
+        <v>0.1366613794446338</v>
+      </c>
+      <c r="H71" t="s">
         <v>231</v>
-      </c>
-      <c r="H71">
-        <v>0.1366613794446338</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2935,11 +2935,11 @@
       <c r="F72">
         <v>1</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72">
+        <v>0.04046133891800937</v>
+      </c>
+      <c r="H72" t="s">
         <v>230</v>
-      </c>
-      <c r="H72">
-        <v>0.04046133891800937</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2961,11 +2961,11 @@
       <c r="F73">
         <v>1</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73">
+        <v>0.03379797915054783</v>
+      </c>
+      <c r="H73" t="s">
         <v>231</v>
-      </c>
-      <c r="H73">
-        <v>0.03379797915054783</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2987,11 +2987,11 @@
       <c r="F74">
         <v>1</v>
       </c>
-      <c r="G74" t="s">
-        <v>228</v>
-      </c>
-      <c r="H74">
+      <c r="G74">
         <v>0.0493285602977285</v>
+      </c>
+      <c r="H74" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3013,11 +3013,11 @@
       <c r="F75">
         <v>1</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75">
+        <v>0.2535656097453243</v>
+      </c>
+      <c r="H75" t="s">
         <v>229</v>
-      </c>
-      <c r="H75">
-        <v>0.2535656097453243</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3039,11 +3039,11 @@
       <c r="F76">
         <v>1</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76">
+        <v>0.1954968605456482</v>
+      </c>
+      <c r="H76" t="s">
         <v>230</v>
-      </c>
-      <c r="H76">
-        <v>0.1954968605456482</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3065,11 +3065,11 @@
       <c r="F77">
         <v>1</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G77">
+        <v>0.09675141504657264</v>
+      </c>
+      <c r="H77" t="s">
         <v>231</v>
-      </c>
-      <c r="H77">
-        <v>0.09675141504657264</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3091,11 +3091,11 @@
       <c r="F78">
         <v>1</v>
       </c>
-      <c r="G78" t="s">
-        <v>228</v>
-      </c>
-      <c r="H78">
+      <c r="G78">
         <v>0.07082135593881524</v>
+      </c>
+      <c r="H78" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3117,11 +3117,11 @@
       <c r="F79">
         <v>1</v>
       </c>
-      <c r="G79" t="s">
-        <v>228</v>
-      </c>
-      <c r="H79">
+      <c r="G79">
         <v>0.03619859082638473</v>
+      </c>
+      <c r="H79" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3143,11 +3143,11 @@
       <c r="F80">
         <v>1</v>
       </c>
-      <c r="G80" t="s">
-        <v>228</v>
-      </c>
-      <c r="H80">
+      <c r="G80">
         <v>0.03101263345522269</v>
+      </c>
+      <c r="H80" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3169,11 +3169,11 @@
       <c r="F81">
         <v>1</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81">
+        <v>0.1964528901908476</v>
+      </c>
+      <c r="H81" t="s">
         <v>230</v>
-      </c>
-      <c r="H81">
-        <v>0.1964528901908476</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3195,11 +3195,11 @@
       <c r="F82">
         <v>1</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82">
+        <v>0.2297296149973506</v>
+      </c>
+      <c r="H82" t="s">
         <v>231</v>
-      </c>
-      <c r="H82">
-        <v>0.2297296149973506</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3221,11 +3221,11 @@
       <c r="F83">
         <v>1</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83">
+        <v>0.08958513629817901</v>
+      </c>
+      <c r="H83" t="s">
         <v>231</v>
-      </c>
-      <c r="H83">
-        <v>0.08958513629817901</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -3247,11 +3247,11 @@
       <c r="F84">
         <v>1</v>
       </c>
-      <c r="G84" t="s">
-        <v>228</v>
-      </c>
-      <c r="H84">
+      <c r="G84">
         <v>0.01875512591595503</v>
+      </c>
+      <c r="H84" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3273,11 +3273,11 @@
       <c r="F85">
         <v>1</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85">
+        <v>0.2535656097453242</v>
+      </c>
+      <c r="H85" t="s">
         <v>229</v>
-      </c>
-      <c r="H85">
-        <v>0.2535656097453242</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3299,11 +3299,11 @@
       <c r="F86">
         <v>1</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86">
+        <v>0.2140962469836062</v>
+      </c>
+      <c r="H86" t="s">
         <v>230</v>
-      </c>
-      <c r="H86">
-        <v>0.2140962469836062</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -3325,11 +3325,11 @@
       <c r="F87">
         <v>1</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87">
+        <v>0.09232342103169502</v>
+      </c>
+      <c r="H87" t="s">
         <v>231</v>
-      </c>
-      <c r="H87">
-        <v>0.09232342103169502</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -3351,11 +3351,11 @@
       <c r="F88">
         <v>1</v>
       </c>
-      <c r="G88" t="s">
-        <v>228</v>
-      </c>
-      <c r="H88">
+      <c r="G88">
         <v>0.04987368511349691</v>
+      </c>
+      <c r="H88" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3377,11 +3377,11 @@
       <c r="F89">
         <v>1</v>
       </c>
-      <c r="G89" t="s">
-        <v>228</v>
-      </c>
-      <c r="H89">
+      <c r="G89">
         <v>0.02932370485801604</v>
+      </c>
+      <c r="H89" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3403,11 +3403,11 @@
       <c r="F90">
         <v>1</v>
       </c>
-      <c r="G90" t="s">
-        <v>228</v>
-      </c>
-      <c r="H90">
+      <c r="G90">
         <v>0.02743626901990923</v>
+      </c>
+      <c r="H90" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -3429,11 +3429,11 @@
       <c r="F91">
         <v>1</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91">
+        <v>0.2212058704541612</v>
+      </c>
+      <c r="H91" t="s">
         <v>230</v>
-      </c>
-      <c r="H91">
-        <v>0.2212058704541612</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3455,11 +3455,11 @@
       <c r="F92">
         <v>1</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92">
+        <v>0.1847766682347926</v>
+      </c>
+      <c r="H92" t="s">
         <v>231</v>
-      </c>
-      <c r="H92">
-        <v>0.1847766682347926</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -3481,11 +3481,11 @@
       <c r="F93">
         <v>1</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93">
+        <v>0.1266196266894915</v>
+      </c>
+      <c r="H93" t="s">
         <v>231</v>
-      </c>
-      <c r="H93">
-        <v>0.1266196266894915</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3507,11 +3507,11 @@
       <c r="F94">
         <v>1</v>
       </c>
-      <c r="G94" t="s">
-        <v>228</v>
-      </c>
-      <c r="H94">
+      <c r="G94">
         <v>0.01758686792936815</v>
+      </c>
+      <c r="H94" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3533,11 +3533,11 @@
       <c r="F95">
         <v>1</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G95">
+        <v>0.1964528901908476</v>
+      </c>
+      <c r="H95" t="s">
         <v>230</v>
-      </c>
-      <c r="H95">
-        <v>0.1964528901908476</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -3559,11 +3559,11 @@
       <c r="F96">
         <v>1</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96">
+        <v>0.1372222209411865</v>
+      </c>
+      <c r="H96" t="s">
         <v>231</v>
-      </c>
-      <c r="H96">
-        <v>0.1372222209411865</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -3585,11 +3585,11 @@
       <c r="F97">
         <v>1</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G97">
+        <v>0.05287871411031179</v>
+      </c>
+      <c r="H97" t="s">
         <v>231</v>
-      </c>
-      <c r="H97">
-        <v>0.05287871411031179</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -3611,11 +3611,11 @@
       <c r="F98">
         <v>1</v>
       </c>
-      <c r="G98" t="s">
-        <v>228</v>
-      </c>
-      <c r="H98">
+      <c r="G98">
         <v>0.02253845474473112</v>
+      </c>
+      <c r="H98" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -3637,11 +3637,11 @@
       <c r="F99">
         <v>1</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99">
+        <v>0.07797341867570605</v>
+      </c>
+      <c r="H99" t="s">
         <v>231</v>
-      </c>
-      <c r="H99">
-        <v>0.07797341867570605</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -3663,11 +3663,11 @@
       <c r="F100">
         <v>1</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G100">
+        <v>0.2535656097453243</v>
+      </c>
+      <c r="H100" t="s">
         <v>229</v>
-      </c>
-      <c r="H100">
-        <v>0.2535656097453243</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3689,11 +3689,11 @@
       <c r="F101">
         <v>1</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G101">
+        <v>0.2140962469836061</v>
+      </c>
+      <c r="H101" t="s">
         <v>230</v>
-      </c>
-      <c r="H101">
-        <v>0.2140962469836061</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3715,11 +3715,11 @@
       <c r="F102">
         <v>1</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G102">
+        <v>0.09232342103169501</v>
+      </c>
+      <c r="H102" t="s">
         <v>231</v>
-      </c>
-      <c r="H102">
-        <v>0.09232342103169501</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3741,11 +3741,11 @@
       <c r="F103">
         <v>1</v>
       </c>
-      <c r="G103" t="s">
-        <v>228</v>
-      </c>
-      <c r="H103">
+      <c r="G103">
         <v>0.05997139061640303</v>
+      </c>
+      <c r="H103" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3767,11 +3767,11 @@
       <c r="F104">
         <v>1</v>
       </c>
-      <c r="G104" t="s">
-        <v>228</v>
-      </c>
-      <c r="H104">
+      <c r="G104">
         <v>0.03229187654282509</v>
+      </c>
+      <c r="H104" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -3793,11 +3793,11 @@
       <c r="F105">
         <v>1</v>
       </c>
-      <c r="G105" t="s">
-        <v>228</v>
-      </c>
-      <c r="H105">
+      <c r="G105">
         <v>0.0322985643492865</v>
+      </c>
+      <c r="H105" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -3819,11 +3819,11 @@
       <c r="F106">
         <v>1</v>
       </c>
-      <c r="G106" t="s">
+      <c r="G106">
+        <v>0.2212058704541612</v>
+      </c>
+      <c r="H106" t="s">
         <v>230</v>
-      </c>
-      <c r="H106">
-        <v>0.2212058704541612</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3845,11 +3845,11 @@
       <c r="F107">
         <v>1</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G107">
+        <v>0.1847766682347927</v>
+      </c>
+      <c r="H107" t="s">
         <v>231</v>
-      </c>
-      <c r="H107">
-        <v>0.1847766682347927</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3871,11 +3871,11 @@
       <c r="F108">
         <v>1</v>
       </c>
-      <c r="G108" t="s">
+      <c r="G108">
+        <v>0.1266196266894915</v>
+      </c>
+      <c r="H108" t="s">
         <v>231</v>
-      </c>
-      <c r="H108">
-        <v>0.1266196266894915</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -3897,11 +3897,11 @@
       <c r="F109">
         <v>1</v>
       </c>
-      <c r="G109" t="s">
-        <v>228</v>
-      </c>
-      <c r="H109">
+      <c r="G109">
         <v>0.01826702356826402</v>
+      </c>
+      <c r="H109" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3923,11 +3923,11 @@
       <c r="F110">
         <v>1</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G110">
+        <v>0.1964528901908477</v>
+      </c>
+      <c r="H110" t="s">
         <v>230</v>
-      </c>
-      <c r="H110">
-        <v>0.1964528901908477</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -3949,11 +3949,11 @@
       <c r="F111">
         <v>1</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G111">
+        <v>0.1372222209411866</v>
+      </c>
+      <c r="H111" t="s">
         <v>231</v>
-      </c>
-      <c r="H111">
-        <v>0.1372222209411866</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3975,11 +3975,11 @@
       <c r="F112">
         <v>1</v>
       </c>
-      <c r="G112" t="s">
+      <c r="G112">
+        <v>0.05287871411031182</v>
+      </c>
+      <c r="H112" t="s">
         <v>231</v>
-      </c>
-      <c r="H112">
-        <v>0.05287871411031182</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4001,11 +4001,11 @@
       <c r="F113">
         <v>1</v>
       </c>
-      <c r="G113" t="s">
-        <v>228</v>
-      </c>
-      <c r="H113">
+      <c r="G113">
         <v>0.02731993540793307</v>
+      </c>
+      <c r="H113" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4027,11 +4027,11 @@
       <c r="F114">
         <v>1</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G114">
+        <v>0.07797341867570602</v>
+      </c>
+      <c r="H114" t="s">
         <v>231</v>
-      </c>
-      <c r="H114">
-        <v>0.07797341867570602</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4053,11 +4053,11 @@
       <c r="F115">
         <v>1</v>
       </c>
-      <c r="G115" t="s">
+      <c r="G115">
+        <v>0.2212058704541612</v>
+      </c>
+      <c r="H115" t="s">
         <v>230</v>
-      </c>
-      <c r="H115">
-        <v>0.2212058704541612</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4079,11 +4079,11 @@
       <c r="F116">
         <v>1</v>
       </c>
-      <c r="G116" t="s">
+      <c r="G116">
+        <v>0.1133135143084126</v>
+      </c>
+      <c r="H116" t="s">
         <v>231</v>
-      </c>
-      <c r="H116">
-        <v>0.1133135143084126</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4105,11 +4105,11 @@
       <c r="F117">
         <v>1</v>
       </c>
-      <c r="G117" t="s">
+      <c r="G117">
+        <v>0.0730007157558778</v>
+      </c>
+      <c r="H117" t="s">
         <v>231</v>
-      </c>
-      <c r="H117">
-        <v>0.0730007157558778</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4131,11 +4131,11 @@
       <c r="F118">
         <v>1</v>
       </c>
-      <c r="G118" t="s">
-        <v>228</v>
-      </c>
-      <c r="H118">
+      <c r="G118">
         <v>0.0205955461179652</v>
+      </c>
+      <c r="H118" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4157,11 +4157,11 @@
       <c r="F119">
         <v>1</v>
       </c>
-      <c r="G119" t="s">
+      <c r="G119">
+        <v>0.08537856111590646</v>
+      </c>
+      <c r="H119" t="s">
         <v>231</v>
-      </c>
-      <c r="H119">
-        <v>0.08537856111590646</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4183,11 +4183,11 @@
       <c r="F120">
         <v>1</v>
       </c>
-      <c r="G120" t="s">
+      <c r="G120">
+        <v>0.04750363786893989</v>
+      </c>
+      <c r="H120" t="s">
         <v>231</v>
-      </c>
-      <c r="H120">
-        <v>0.04750363786893989</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4209,11 +4209,11 @@
       <c r="F121">
         <v>1</v>
       </c>
-      <c r="G121" t="s">
+      <c r="G121">
+        <v>0.2212058704541612</v>
+      </c>
+      <c r="H121" t="s">
         <v>230</v>
-      </c>
-      <c r="H121">
-        <v>0.2212058704541612</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4235,11 +4235,11 @@
       <c r="F122">
         <v>1</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G122">
+        <v>0.1133135143084126</v>
+      </c>
+      <c r="H122" t="s">
         <v>231</v>
-      </c>
-      <c r="H122">
-        <v>0.1133135143084126</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4261,11 +4261,11 @@
       <c r="F123">
         <v>1</v>
       </c>
-      <c r="G123" t="s">
+      <c r="G123">
+        <v>0.0730007157558778</v>
+      </c>
+      <c r="H123" t="s">
         <v>231</v>
-      </c>
-      <c r="H123">
-        <v>0.0730007157558778</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4287,11 +4287,11 @@
       <c r="F124">
         <v>1</v>
       </c>
-      <c r="G124" t="s">
-        <v>228</v>
-      </c>
-      <c r="H124">
+      <c r="G124">
         <v>0.02418748432187934</v>
+      </c>
+      <c r="H124" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -4313,11 +4313,11 @@
       <c r="F125">
         <v>1</v>
       </c>
-      <c r="G125" t="s">
+      <c r="G125">
+        <v>0.08537856111590647</v>
+      </c>
+      <c r="H125" t="s">
         <v>231</v>
-      </c>
-      <c r="H125">
-        <v>0.08537856111590647</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -4339,11 +4339,11 @@
       <c r="F126">
         <v>1</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G126">
+        <v>0.04750363786893992</v>
+      </c>
+      <c r="H126" t="s">
         <v>231</v>
-      </c>
-      <c r="H126">
-        <v>0.04750363786893992</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -4365,11 +4365,11 @@
       <c r="F127">
         <v>1</v>
       </c>
-      <c r="G127" t="s">
+      <c r="G127">
+        <v>0.05571833687102554</v>
+      </c>
+      <c r="H127" t="s">
         <v>231</v>
-      </c>
-      <c r="H127">
-        <v>0.05571833687102554</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -4391,11 +4391,11 @@
       <c r="F128">
         <v>1</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G128">
+        <v>0.05571833687102553</v>
+      </c>
+      <c r="H128" t="s">
         <v>231</v>
-      </c>
-      <c r="H128">
-        <v>0.05571833687102553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final hyp gen data
</commit_message>
<xml_diff>
--- a/refined-hyp-data-3.xlsx
+++ b/refined-hyp-data-3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="228">
   <si>
     <t>True Nodes</t>
   </si>
@@ -34,9 +34,6 @@
     <t>P(H|O)</t>
   </si>
   <si>
-    <t>Best Explanation (flipped)</t>
-  </si>
-  <si>
     <t>['B1']</t>
   </si>
   <si>
@@ -701,15 +698,6 @@
   </si>
   <si>
     <t>H1</t>
-  </si>
-  <si>
-    <t>['H1', 'H2', 'H3']</t>
-  </si>
-  <si>
-    <t>['H1', 'H3', 'H4']</t>
-  </si>
-  <si>
-    <t>['H1']</t>
   </si>
 </sst>
 </file>
@@ -1067,13 +1055,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1092,25 +1080,22 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1118,25 +1103,22 @@
       <c r="G2">
         <v>0.0822123787580261</v>
       </c>
-      <c r="H2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1144,25 +1126,22 @@
       <c r="G3">
         <v>0.06790001332745053</v>
       </c>
-      <c r="H3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1170,77 +1149,68 @@
       <c r="G4">
         <v>0.05468171459519593</v>
       </c>
-      <c r="H4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0.2629514961735958</v>
-      </c>
-      <c r="H5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.09798693680418633</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.04547141860584613</v>
-      </c>
-      <c r="H6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.02857923041736947</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1248,25 +1218,22 @@
       <c r="G7">
         <v>0.06063476235243403</v>
       </c>
-      <c r="H7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1274,25 +1241,22 @@
       <c r="G8">
         <v>0.04030129522014882</v>
       </c>
-      <c r="H8" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1300,25 +1264,22 @@
       <c r="G9">
         <v>0.086901769271174</v>
       </c>
-      <c r="H9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1326,77 +1287,68 @@
       <c r="G10">
         <v>0.06354147988076518</v>
       </c>
-      <c r="H10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0.2629514961735958</v>
-      </c>
-      <c r="H11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>0.1060100375094771</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0.04547141860584613</v>
-      </c>
-      <c r="H12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>0.03192009104625149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1404,25 +1356,22 @@
       <c r="G13">
         <v>0.07745045519474988</v>
       </c>
-      <c r="H13" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1430,25 +1379,22 @@
       <c r="G14">
         <v>0.04561744588877638</v>
       </c>
-      <c r="H14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1456,77 +1402,68 @@
       <c r="G15">
         <v>0.06206522356065326</v>
       </c>
-      <c r="H15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
-        <v>0.2629514961735958</v>
-      </c>
-      <c r="H16" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>0.0993902443089265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0.04547141860584613</v>
-      </c>
-      <c r="H17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>0.02866096023323091</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1534,25 +1471,22 @@
       <c r="G18">
         <v>0.05858210392112535</v>
       </c>
-      <c r="H18" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1560,51 +1494,45 @@
       <c r="G19">
         <v>0.04380767160551077</v>
       </c>
-      <c r="H19" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0.268207609833135</v>
-      </c>
-      <c r="H20" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>0.1243001434716429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1612,25 +1540,22 @@
       <c r="G21">
         <v>0.04886924445435459</v>
       </c>
-      <c r="H21" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1638,25 +1563,22 @@
       <c r="G22">
         <v>0.04363957256688109</v>
       </c>
-      <c r="H22" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1664,155 +1586,137 @@
       <c r="G23">
         <v>0.02865844532533962</v>
       </c>
-      <c r="H23" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>0.248596438043593</v>
-      </c>
-      <c r="H24" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>0.07382431753584227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25">
-        <v>0.1954968605456482</v>
-      </c>
-      <c r="H25" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>0.08980581761832562</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
-        <v>0.1361480655135886</v>
-      </c>
-      <c r="H26" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>0.09994812983051261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27">
-        <v>0.03593370716208692</v>
-      </c>
-      <c r="H27" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>0.02692810663547745</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
-        <v>0.04202043911776646</v>
-      </c>
-      <c r="H28" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>0.03304253383339509</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1820,25 +1724,22 @@
       <c r="G29">
         <v>0.04264444475012164</v>
       </c>
-      <c r="H29" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1846,77 +1747,68 @@
       <c r="G30">
         <v>0.07464945633127076</v>
       </c>
-      <c r="H30" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31">
-        <v>0.2629514961735958</v>
-      </c>
-      <c r="H31" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>0.1094276445899048</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32">
-        <v>0.04547141860584612</v>
-      </c>
-      <c r="H32" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>0.03315611827294026</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1924,25 +1816,22 @@
       <c r="G33">
         <v>0.07350696097347734</v>
       </c>
-      <c r="H33" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1950,51 +1839,45 @@
       <c r="G34">
         <v>0.05030197306018955</v>
       </c>
-      <c r="H34" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35">
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35">
-        <v>0.2682076098331351</v>
-      </c>
-      <c r="H35" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>0.1124399336365382</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2002,25 +1885,22 @@
       <c r="G36">
         <v>0.05525483750915555</v>
       </c>
-      <c r="H36" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2028,25 +1908,22 @@
       <c r="G37">
         <v>0.05290772104811078</v>
       </c>
-      <c r="H37" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2054,155 +1931,137 @@
       <c r="G38">
         <v>0.03244283555361271</v>
       </c>
-      <c r="H38" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39">
-        <v>0.248596438043593</v>
-      </c>
-      <c r="H39" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>0.06363350235252514</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E40" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40">
-        <v>0.1954968605456481</v>
-      </c>
-      <c r="H40" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>0.09829596123523733</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41">
-        <v>0.1361480655135885</v>
-      </c>
-      <c r="H41" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>0.08745020379511895</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42">
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="G42">
-        <v>0.03593370716208692</v>
-      </c>
-      <c r="H42" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>0.03189094266261995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43">
-        <v>0.04202043911776644</v>
-      </c>
-      <c r="H43" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>0.02994293727114758</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44">
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -2210,77 +2069,68 @@
       <c r="G44">
         <v>0.05171001288247373</v>
       </c>
-      <c r="H44" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45">
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
       <c r="G45">
-        <v>0.268207609833135</v>
-      </c>
-      <c r="H45" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>0.1237171201389319</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46">
-        <v>0.04638034267713199</v>
-      </c>
-      <c r="H46" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>0.04565951575645399</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2288,25 +2138,22 @@
       <c r="G47">
         <v>0.04667334377643362</v>
       </c>
-      <c r="H47" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -2314,155 +2161,137 @@
       <c r="G48">
         <v>0.03272729337207169</v>
       </c>
-      <c r="H48" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49">
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F49">
         <v>1</v>
       </c>
       <c r="G49">
-        <v>0.248596438043593</v>
-      </c>
-      <c r="H49" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>0.06617175554166629</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50">
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="G50">
-        <v>0.2140962469836062</v>
-      </c>
-      <c r="H50" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>0.09584405647954954</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51">
-        <v>0.1366613794446337</v>
-      </c>
-      <c r="H51" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>0.1037281262128822</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E52" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F52">
         <v>1</v>
       </c>
       <c r="G52">
-        <v>0.04046133891800937</v>
-      </c>
-      <c r="H52" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>0.02562114792661457</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53">
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E53" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F53">
         <v>1</v>
       </c>
       <c r="G53">
-        <v>0.03379797915054781</v>
-      </c>
-      <c r="H53" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>0.0295831298909644</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E54" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -2470,103 +2299,91 @@
       <c r="G54">
         <v>0.04261268674073516</v>
       </c>
-      <c r="H54" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C55">
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55">
-        <v>0.2535656097453242</v>
-      </c>
-      <c r="H55" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>0.1216142039073001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C56">
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56">
-        <v>0.1954968605456481</v>
-      </c>
-      <c r="H56" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>0.08410429382729084</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57">
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F57">
         <v>1</v>
       </c>
       <c r="G57">
-        <v>0.09675141504657259</v>
-      </c>
-      <c r="H57" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+        <v>0.07104577694263146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E58" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2574,25 +2391,22 @@
       <c r="G58">
         <v>0.05708123659060638</v>
       </c>
-      <c r="H58" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -2600,25 +2414,22 @@
       <c r="G59">
         <v>0.03335013995169677</v>
       </c>
-      <c r="H59" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E60" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2626,103 +2437,91 @@
       <c r="G60">
         <v>0.02553577334619476</v>
       </c>
-      <c r="H60" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61">
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E61" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="G61">
-        <v>0.1964528901908476</v>
-      </c>
-      <c r="H61" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>0.05709136848068581</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62">
         <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="G62">
-        <v>0.2297296149973507</v>
-      </c>
-      <c r="H62" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>0.1331797727244467</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63">
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
       <c r="G63">
-        <v>0.08958513629817907</v>
-      </c>
-      <c r="H63" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>0.08212622969824161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64">
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2730,51 +2529,45 @@
       <c r="G64">
         <v>0.01760208236291312</v>
       </c>
-      <c r="H64" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65">
         <v>4</v>
       </c>
       <c r="D65" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F65">
         <v>1</v>
       </c>
       <c r="G65">
-        <v>0.268207609833135</v>
-      </c>
-      <c r="H65" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>0.1180812702908866</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C66">
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E66" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2782,25 +2575,22 @@
       <c r="G66">
         <v>0.05228091384282959</v>
       </c>
-      <c r="H66" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C67">
         <v>4</v>
       </c>
       <c r="D67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E67" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2808,25 +2598,22 @@
       <c r="G67">
         <v>0.05562363358634346</v>
       </c>
-      <c r="H67" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68">
         <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E68" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2834,155 +2621,137 @@
       <c r="G68">
         <v>0.03819607002916236</v>
       </c>
-      <c r="H68" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C69">
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E69" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F69">
         <v>1</v>
       </c>
       <c r="G69">
-        <v>0.248596438043593</v>
-      </c>
-      <c r="H69" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>0.05949530033271561</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C70">
         <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F70">
         <v>1</v>
       </c>
       <c r="G70">
-        <v>0.2140962469836062</v>
-      </c>
-      <c r="H70" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+        <v>0.09995590061204046</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C71">
         <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F71">
         <v>1</v>
       </c>
       <c r="G71">
-        <v>0.1366613794446338</v>
-      </c>
-      <c r="H71" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>0.0923580131110586</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C72">
         <v>4</v>
       </c>
       <c r="D72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E72" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F72">
         <v>1</v>
       </c>
       <c r="G72">
-        <v>0.04046133891800937</v>
-      </c>
-      <c r="H72" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+        <v>0.02990901914405578</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C73">
         <v>4</v>
       </c>
       <c r="D73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E73" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F73">
         <v>1</v>
       </c>
       <c r="G73">
-        <v>0.03379797915054783</v>
-      </c>
-      <c r="H73" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <v>0.02812796503217065</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C74">
         <v>4</v>
       </c>
       <c r="D74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -2990,103 +2759,91 @@
       <c r="G74">
         <v>0.0493285602977285</v>
       </c>
-      <c r="H74" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C75">
         <v>4</v>
       </c>
       <c r="D75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E75" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F75">
         <v>1</v>
       </c>
       <c r="G75">
-        <v>0.2535656097453243</v>
-      </c>
-      <c r="H75" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <v>0.1062711802920084</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C76">
         <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E76" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F76">
         <v>1</v>
       </c>
       <c r="G76">
-        <v>0.1954968605456482</v>
-      </c>
-      <c r="H76" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+        <v>0.08144127183936287</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C77">
         <v>4</v>
       </c>
       <c r="D77" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E77" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F77">
         <v>1</v>
       </c>
       <c r="G77">
-        <v>0.09675141504657264</v>
-      </c>
-      <c r="H77" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+        <v>0.06217097764662466</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C78">
         <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E78" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -3094,25 +2851,22 @@
       <c r="G78">
         <v>0.07082135593881524</v>
       </c>
-      <c r="H78" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C79">
         <v>4</v>
       </c>
       <c r="D79" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E79" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -3120,25 +2874,22 @@
       <c r="G79">
         <v>0.03619859082638473</v>
       </c>
-      <c r="H79" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C80">
         <v>4</v>
       </c>
       <c r="D80" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E80" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -3146,103 +2897,91 @@
       <c r="G80">
         <v>0.03101263345522269</v>
       </c>
-      <c r="H80" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C81">
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E81" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F81">
         <v>1</v>
       </c>
       <c r="G81">
-        <v>0.1964528901908476</v>
-      </c>
-      <c r="H81" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
+        <v>0.05310753191349251</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C82">
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E82" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
       <c r="G82">
-        <v>0.2297296149973506</v>
-      </c>
-      <c r="H82" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+        <v>0.09984621108445156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C83">
         <v>4</v>
       </c>
       <c r="D83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E83" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="G83">
-        <v>0.08958513629817901</v>
-      </c>
-      <c r="H83" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
+        <v>0.07955106316184052</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C84">
         <v>4</v>
       </c>
       <c r="D84" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -3250,103 +2989,91 @@
       <c r="G84">
         <v>0.01875512591595503</v>
       </c>
-      <c r="H84" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C85">
         <v>4</v>
       </c>
       <c r="D85" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E85" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F85">
         <v>1</v>
       </c>
       <c r="G85">
-        <v>0.2535656097453242</v>
-      </c>
-      <c r="H85" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>0.1091256993812344</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C86">
         <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E86" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F86">
         <v>1</v>
       </c>
       <c r="G86">
-        <v>0.2140962469836062</v>
-      </c>
-      <c r="H86" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+        <v>0.09656063535626422</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C87">
         <v>4</v>
       </c>
       <c r="D87" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E87" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F87">
         <v>1</v>
       </c>
       <c r="G87">
-        <v>0.09232342103169502</v>
-      </c>
-      <c r="H87" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+        <v>0.07325286764385974</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C88">
         <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E88" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -3354,25 +3081,22 @@
       <c r="G88">
         <v>0.04987368511349691</v>
       </c>
-      <c r="H88" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C89">
         <v>4</v>
       </c>
       <c r="D89" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E89" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -3380,25 +3104,22 @@
       <c r="G89">
         <v>0.02932370485801604</v>
       </c>
-      <c r="H89" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C90">
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E90" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -3406,103 +3127,91 @@
       <c r="G90">
         <v>0.02743626901990923</v>
       </c>
-      <c r="H90" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C91">
         <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E91" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F91">
         <v>1</v>
       </c>
       <c r="G91">
-        <v>0.2212058704541612</v>
-      </c>
-      <c r="H91" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <v>0.05730238410889727</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C92">
         <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F92">
         <v>1</v>
       </c>
       <c r="G92">
-        <v>0.1847766682347926</v>
-      </c>
-      <c r="H92" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <v>0.1101694287286829</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C93">
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F93">
         <v>1</v>
       </c>
       <c r="G93">
-        <v>0.1266196266894915</v>
-      </c>
-      <c r="H93" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+        <v>0.09815964704036267</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C94">
         <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E94" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -3510,103 +3219,91 @@
       <c r="G94">
         <v>0.01758686792936815</v>
       </c>
-      <c r="H94" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C95">
         <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F95">
         <v>1</v>
       </c>
       <c r="G95">
-        <v>0.1964528901908476</v>
-      </c>
-      <c r="H95" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>0.09890029158345161</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C96">
         <v>4</v>
       </c>
       <c r="D96" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E96" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F96">
         <v>1</v>
       </c>
       <c r="G96">
-        <v>0.1372222209411865</v>
-      </c>
-      <c r="H96" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <v>0.09336195354021604</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C97">
         <v>4</v>
       </c>
       <c r="D97" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E97" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F97">
         <v>1</v>
       </c>
       <c r="G97">
-        <v>0.05287871411031179</v>
-      </c>
-      <c r="H97" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
+        <v>0.04884567003728634</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C98">
         <v>4</v>
       </c>
       <c r="D98" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -3614,129 +3311,114 @@
       <c r="G98">
         <v>0.02253845474473112</v>
       </c>
-      <c r="H98" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C99">
         <v>4</v>
       </c>
       <c r="D99" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E99" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F99">
         <v>1</v>
       </c>
       <c r="G99">
-        <v>0.07797341867570605</v>
-      </c>
-      <c r="H99" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
+        <v>0.05168284573275966</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C100">
         <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E100" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F100">
         <v>1</v>
       </c>
       <c r="G100">
-        <v>0.2535656097453243</v>
-      </c>
-      <c r="H100" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+        <v>0.09681857971886049</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C101">
         <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E101" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F101">
         <v>1</v>
       </c>
       <c r="G101">
-        <v>0.2140962469836061</v>
-      </c>
-      <c r="H101" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
+        <v>0.09073412986219737</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C102">
         <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E102" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F102">
         <v>1</v>
       </c>
       <c r="G102">
-        <v>0.09232342103169501</v>
-      </c>
-      <c r="H102" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
+        <v>0.06666881269465119</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C103">
         <v>5</v>
       </c>
       <c r="D103" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E103" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -3744,25 +3426,22 @@
       <c r="G103">
         <v>0.05997139061640303</v>
       </c>
-      <c r="H103" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C104">
         <v>5</v>
       </c>
       <c r="D104" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E104" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3770,25 +3449,22 @@
       <c r="G104">
         <v>0.03229187654282509</v>
       </c>
-      <c r="H104" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C105">
         <v>5</v>
       </c>
       <c r="D105" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E105" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3796,103 +3472,91 @@
       <c r="G105">
         <v>0.0322985643492865</v>
       </c>
-      <c r="H105" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C106">
         <v>5</v>
       </c>
       <c r="D106" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E106" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F106">
         <v>1</v>
       </c>
       <c r="G106">
-        <v>0.2212058704541612</v>
-      </c>
-      <c r="H106" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
+        <v>0.05216818747607118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" s="1">
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C107">
         <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E107" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F107">
         <v>1</v>
       </c>
       <c r="G107">
-        <v>0.1847766682347927</v>
-      </c>
-      <c r="H107" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
+        <v>0.08441148901255856</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108" s="1">
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C108">
         <v>5</v>
       </c>
       <c r="D108" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E108" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F108">
         <v>1</v>
       </c>
       <c r="G108">
-        <v>0.1266196266894915</v>
-      </c>
-      <c r="H108" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
+        <v>0.08833391906842303</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" s="1">
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C109">
         <v>5</v>
       </c>
       <c r="D109" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E109" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -3900,103 +3564,91 @@
       <c r="G109">
         <v>0.01826702356826402</v>
       </c>
-      <c r="H109" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110" s="1">
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C110">
         <v>5</v>
       </c>
       <c r="D110" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E110" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F110">
         <v>1</v>
       </c>
       <c r="G110">
-        <v>0.1964528901908477</v>
-      </c>
-      <c r="H110" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
+        <v>0.1004231064377551</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" s="1">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C111">
         <v>5</v>
       </c>
       <c r="D111" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E111" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F111">
         <v>1</v>
       </c>
       <c r="G111">
-        <v>0.1372222209411866</v>
-      </c>
-      <c r="H111" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
+        <v>0.07821931951265913</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112" s="1">
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C112">
         <v>5</v>
       </c>
       <c r="D112" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E112" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F112">
         <v>1</v>
       </c>
       <c r="G112">
-        <v>0.05287871411031182</v>
-      </c>
-      <c r="H112" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8">
+        <v>0.04745327290809138</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113" s="1">
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C113">
         <v>5</v>
       </c>
       <c r="D113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E113" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -4004,129 +3656,114 @@
       <c r="G113">
         <v>0.02731993540793307</v>
       </c>
-      <c r="H113" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8">
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114" s="1">
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C114">
         <v>5</v>
       </c>
       <c r="D114" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E114" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F114">
         <v>1</v>
       </c>
       <c r="G114">
-        <v>0.07797341867570602</v>
-      </c>
-      <c r="H114" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8">
+        <v>0.04260609932785706</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115" s="1">
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C115">
         <v>5</v>
       </c>
       <c r="D115" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E115" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F115">
         <v>1</v>
       </c>
       <c r="G115">
-        <v>0.2212058704541612</v>
-      </c>
-      <c r="H115" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
+        <v>0.09951547791325453</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116" s="1">
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C116">
         <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E116" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F116">
         <v>1</v>
       </c>
       <c r="G116">
-        <v>0.1133135143084126</v>
-      </c>
-      <c r="H116" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8">
+        <v>0.07890537400780157</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117" s="1">
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C117">
         <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E117" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F117">
         <v>1</v>
       </c>
       <c r="G117">
-        <v>0.0730007157558778</v>
-      </c>
-      <c r="H117" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8">
+        <v>0.05950274256610904</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118" s="1">
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C118">
         <v>5</v>
       </c>
       <c r="D118" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F118">
         <v>1</v>
@@ -4134,155 +3771,137 @@
       <c r="G118">
         <v>0.0205955461179652</v>
       </c>
-      <c r="H118" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8">
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" s="1">
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C119">
         <v>5</v>
       </c>
       <c r="D119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E119" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F119">
         <v>1</v>
       </c>
       <c r="G119">
-        <v>0.08537856111590646</v>
-      </c>
-      <c r="H119" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8">
+        <v>0.05487977600403231</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120" s="1">
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C120">
         <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E120" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F120">
         <v>1</v>
       </c>
       <c r="G120">
-        <v>0.04750363786893989</v>
-      </c>
-      <c r="H120" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8">
+        <v>0.04347308511518126</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121" s="1">
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C121">
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E121" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F121">
         <v>1</v>
       </c>
       <c r="G121">
-        <v>0.2212058704541612</v>
-      </c>
-      <c r="H121" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8">
+        <v>0.09494151233372046</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122" s="1">
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C122">
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E122" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F122">
         <v>1</v>
       </c>
       <c r="G122">
-        <v>0.1133135143084126</v>
-      </c>
-      <c r="H122" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8">
+        <v>0.06702606029140937</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
       <c r="A123" s="1">
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C123">
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E123" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F123">
         <v>1</v>
       </c>
       <c r="G123">
-        <v>0.0730007157558778</v>
-      </c>
-      <c r="H123" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8">
+        <v>0.05484260526558004</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
       <c r="A124" s="1">
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C124">
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E124" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F124">
         <v>1</v>
@@ -4290,112 +3909,97 @@
       <c r="G124">
         <v>0.02418748432187934</v>
       </c>
-      <c r="H124" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8">
+    </row>
+    <row r="125" spans="1:7">
       <c r="A125" s="1">
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C125">
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E125" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F125">
         <v>1</v>
       </c>
       <c r="G125">
-        <v>0.08537856111590647</v>
-      </c>
-      <c r="H125" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8">
+        <v>0.04435015617722782</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
       <c r="A126" s="1">
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C126">
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E126" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F126">
         <v>1</v>
       </c>
       <c r="G126">
-        <v>0.04750363786893992</v>
-      </c>
-      <c r="H126" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8">
+        <v>0.04208154810696001</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
       <c r="A127" s="1">
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C127">
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E127" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F127">
         <v>1</v>
       </c>
       <c r="G127">
-        <v>0.05571833687102554</v>
-      </c>
-      <c r="H127" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
+        <v>0.04506550141754449</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
       <c r="A128" s="1">
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C128">
         <v>7</v>
       </c>
       <c r="D128" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E128" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F128">
         <v>1</v>
       </c>
       <c r="G128">
-        <v>0.05571833687102553</v>
-      </c>
-      <c r="H128" t="s">
-        <v>231</v>
+        <v>0.04138763992269474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>